<commit_message>
Blosum based protein similarity calculation
</commit_message>
<xml_diff>
--- a/kuzmin analysis/Nearest Neighbor/human_CoV2_sims.xlsx
+++ b/kuzmin analysis/Nearest Neighbor/human_CoV2_sims.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NBOLLIG\Desktop\machine-mutation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D75F29D-7158-49D1-8BAE-057CD34C39B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2CE21B0A-2E1F-4C54-BBD4-042FFC350510}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440"/>
   </bookViews>
@@ -313,10 +313,10 @@
     <t>QIV15164</t>
   </si>
   <si>
-    <t>before MM</t>
-  </si>
-  <si>
-    <t>after MM</t>
+    <t>sim to bat</t>
+  </si>
+  <si>
+    <t>sim to MM bat</t>
   </si>
   <si>
     <t>diff</t>
@@ -1163,7 +1163,7 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,7 +1171,9 @@
     <col min="1" max="1" width="46" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1187,10 +1189,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -1199,22 +1201,22 @@
         <v>3</v>
       </c>
       <c r="E2">
-        <v>0.92040977147360103</v>
+        <v>0.98514450346628202</v>
       </c>
       <c r="F2">
-        <v>0.75571315996847899</v>
+        <v>0.86206896551724099</v>
       </c>
       <c r="G2">
         <f>F2-E2</f>
-        <v>-0.16469661150512205</v>
+        <v>-0.12307553794904103</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -1223,14 +1225,14 @@
         <v>3</v>
       </c>
       <c r="E3">
-        <v>0.96296296296296202</v>
+        <v>0.99275634995296302</v>
       </c>
       <c r="F3">
-        <v>0.79117415287628001</v>
+        <v>0.86895578551269903</v>
       </c>
       <c r="G3">
         <f>F3-E3</f>
-        <v>-0.17178881008668201</v>
+        <v>-0.12380056444026399</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1247,14 +1249,14 @@
         <v>3</v>
       </c>
       <c r="E4">
-        <v>0.96769109535066899</v>
+        <v>0.98482399425287304</v>
       </c>
       <c r="F4">
-        <v>0.793538219070134</v>
+        <v>0.86054238505747105</v>
       </c>
       <c r="G4">
         <f>F4-E4</f>
-        <v>-0.174152876280535</v>
+        <v>-0.12428160919540199</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1271,22 +1273,22 @@
         <v>3</v>
       </c>
       <c r="E5">
-        <v>0.96926713947990495</v>
+        <v>0.98422090729782996</v>
       </c>
       <c r="F5">
-        <v>0.79511426319936895</v>
+        <v>0.85933297471758996</v>
       </c>
       <c r="G5">
         <f>F5-E5</f>
-        <v>-0.174152876280536</v>
+        <v>-0.12488793258024</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -1295,22 +1297,22 @@
         <v>3</v>
       </c>
       <c r="E6">
-        <v>0.94405043341213501</v>
+        <v>0.98341506910387799</v>
       </c>
       <c r="F6">
-        <v>0.76989755713159902</v>
+        <v>0.858493089612126</v>
       </c>
       <c r="G6">
         <f>F6-E6</f>
-        <v>-0.174152876280536</v>
+        <v>-0.12492197949175199</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -1319,14 +1321,14 @@
         <v>3</v>
       </c>
       <c r="E7">
-        <v>0.97635933806146502</v>
+        <v>0.98403780988050604</v>
       </c>
       <c r="F7">
-        <v>0.80063041765169396</v>
+        <v>0.85910469056536398</v>
       </c>
       <c r="G7">
         <f>F7-E7</f>
-        <v>-0.17572892040977106</v>
+        <v>-0.12493311931514206</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1343,22 +1345,22 @@
         <v>3</v>
       </c>
       <c r="E8">
-        <v>0.97635933806146502</v>
+        <v>0.98457010346057705</v>
       </c>
       <c r="F8">
-        <v>0.79984239558707604</v>
+        <v>0.85961469853728101</v>
       </c>
       <c r="G8">
         <f>F8-E8</f>
-        <v>-0.17651694247438898</v>
+        <v>-0.12495540492329604</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>83</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
@@ -1367,22 +1369,22 @@
         <v>3</v>
       </c>
       <c r="E9">
-        <v>0.97635933806146502</v>
+        <v>0.98457010346057705</v>
       </c>
       <c r="F9">
-        <v>0.79984239558707604</v>
+        <v>0.85961469853728101</v>
       </c>
       <c r="G9">
         <f>F9-E9</f>
-        <v>-0.17651694247438898</v>
+        <v>-0.12495540492329604</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
@@ -1391,22 +1393,22 @@
         <v>3</v>
       </c>
       <c r="E10">
-        <v>0.97557131599684699</v>
+        <v>0.98376449598572702</v>
       </c>
       <c r="F10">
-        <v>0.79905437352245801</v>
+        <v>0.85878679750222997</v>
       </c>
       <c r="G10">
         <f>F10-E10</f>
-        <v>-0.17651694247438898</v>
+        <v>-0.12497769848349705</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -1415,22 +1417,22 @@
         <v>3</v>
       </c>
       <c r="E11">
-        <v>0.97635933806146502</v>
+        <v>0.98421475073575304</v>
       </c>
       <c r="F11">
-        <v>0.79984239558707604</v>
+        <v>0.85918130741104004</v>
       </c>
       <c r="G11">
         <f>F11-E11</f>
-        <v>-0.17651694247438898</v>
+        <v>-0.125033443324713</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
         <v>2</v>
@@ -1439,22 +1441,22 @@
         <v>3</v>
       </c>
       <c r="E12">
-        <v>0.97635933806146502</v>
+        <v>0.98490397498883397</v>
       </c>
       <c r="F12">
-        <v>0.79984239558707604</v>
+        <v>0.85984814649397001</v>
       </c>
       <c r="G12">
         <f>F12-E12</f>
-        <v>-0.17651694247438898</v>
+        <v>-0.12505582849486396</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B13" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
@@ -1463,22 +1465,22 @@
         <v>3</v>
       </c>
       <c r="E13">
-        <v>0.97557131599684699</v>
+        <v>0.98448229733345205</v>
       </c>
       <c r="F13">
-        <v>0.79905437352245801</v>
+        <v>0.85918130741104004</v>
       </c>
       <c r="G13">
         <f>F13-E13</f>
-        <v>-0.17651694247438898</v>
+        <v>-0.12530098992241201</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
@@ -1487,22 +1489,22 @@
         <v>3</v>
       </c>
       <c r="E14">
-        <v>0.97635933806146502</v>
+        <v>0.984572855359372</v>
       </c>
       <c r="F14">
-        <v>0.79984239558707604</v>
+        <v>0.85919386481184201</v>
       </c>
       <c r="G14">
         <f>F14-E14</f>
-        <v>-0.17651694247438898</v>
+        <v>-0.12537899054752999</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>88</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
@@ -1511,22 +1513,22 @@
         <v>3</v>
       </c>
       <c r="E15">
-        <v>0.97635933806146502</v>
+        <v>0.98448229733345205</v>
       </c>
       <c r="F15">
-        <v>0.79984239558707604</v>
+        <v>0.859092125211807</v>
       </c>
       <c r="G15">
         <f>F15-E15</f>
-        <v>-0.17651694247438898</v>
+        <v>-0.12539017212164505</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
@@ -1535,22 +1537,22 @@
         <v>3</v>
       </c>
       <c r="E16">
-        <v>0.97634069400630896</v>
+        <v>0.98369129311113002</v>
       </c>
       <c r="F16">
-        <v>0.79968454258675004</v>
+        <v>0.858123161928526</v>
       </c>
       <c r="G16">
         <f>F16-E16</f>
-        <v>-0.17665615141955893</v>
+        <v>-0.12556813118260401</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -1559,22 +1561,22 @@
         <v>3</v>
       </c>
       <c r="E17">
-        <v>0.97478329393222996</v>
+        <v>0.98395292859053196</v>
       </c>
       <c r="F17">
-        <v>0.79747832939322305</v>
+        <v>0.85834001961308704</v>
       </c>
       <c r="G17">
         <f>F17-E17</f>
-        <v>-0.1773049645390069</v>
+        <v>-0.12561290897744493</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
         <v>2</v>
@@ -1583,22 +1585,22 @@
         <v>3</v>
       </c>
       <c r="E18">
-        <v>0.97635933806146502</v>
+        <v>0.98412981455064197</v>
       </c>
       <c r="F18">
-        <v>0.79905437352245801</v>
+        <v>0.85850570613409405</v>
       </c>
       <c r="G18">
         <f>F18-E18</f>
-        <v>-0.17730496453900702</v>
+        <v>-0.12562410841654792</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>90</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
@@ -1607,22 +1609,22 @@
         <v>3</v>
       </c>
       <c r="E19">
-        <v>0.97635933806146502</v>
+        <v>0.98412981455064197</v>
       </c>
       <c r="F19">
-        <v>0.79905437352245801</v>
+        <v>0.85850570613409405</v>
       </c>
       <c r="G19">
         <f>F19-E19</f>
-        <v>-0.17730496453900702</v>
+        <v>-0.12562410841654792</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
@@ -1631,22 +1633,22 @@
         <v>3</v>
       </c>
       <c r="E20">
-        <v>0.97635933806146502</v>
+        <v>0.98439728958630501</v>
       </c>
       <c r="F20">
-        <v>0.79905437352245801</v>
+        <v>0.85877318116975698</v>
       </c>
       <c r="G20">
         <f>F20-E20</f>
-        <v>-0.17730496453900702</v>
+        <v>-0.12562410841654803</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
+        <v>75</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
@@ -1655,22 +1657,22 @@
         <v>3</v>
       </c>
       <c r="E21">
-        <v>0.97714736012608305</v>
+        <v>0.98377318116975698</v>
       </c>
       <c r="F21">
-        <v>0.79984239558707604</v>
+        <v>0.85814907275320895</v>
       </c>
       <c r="G21">
         <f>F21-E21</f>
-        <v>-0.17730496453900702</v>
+        <v>-0.12562410841654803</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C22" t="s">
         <v>2</v>
@@ -1679,22 +1681,22 @@
         <v>3</v>
       </c>
       <c r="E22">
-        <v>0.97635933806146502</v>
+        <v>0.98439589835042296</v>
       </c>
       <c r="F22">
-        <v>0.79905437352245801</v>
+        <v>0.85876058849754699</v>
       </c>
       <c r="G22">
         <f>F22-E22</f>
-        <v>-0.17730496453900702</v>
+        <v>-0.12563530985287596</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
@@ -1703,22 +1705,22 @@
         <v>3</v>
       </c>
       <c r="E23">
-        <v>0.97793538219070097</v>
+        <v>0.98457423094070395</v>
       </c>
       <c r="F23">
-        <v>0.80063041765169396</v>
+        <v>0.85893892108782799</v>
       </c>
       <c r="G23">
         <f>F23-E23</f>
-        <v>-0.17730496453900702</v>
+        <v>-0.12563530985287596</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="B24" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="C24" t="s">
         <v>2</v>
@@ -1727,22 +1729,22 @@
         <v>3</v>
       </c>
       <c r="E24">
-        <v>0.97635933806146502</v>
+        <v>0.98448506464556396</v>
       </c>
       <c r="F24">
-        <v>0.79905437352245801</v>
+        <v>0.85884975479268799</v>
       </c>
       <c r="G24">
         <f>F24-E24</f>
-        <v>-0.17730496453900702</v>
+        <v>-0.12563530985287596</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="C25" t="s">
         <v>2</v>
@@ -1751,22 +1753,22 @@
         <v>3</v>
       </c>
       <c r="E25">
-        <v>0.97635933806146502</v>
+        <v>0.98466202960584903</v>
       </c>
       <c r="F25">
-        <v>0.79905437352245801</v>
+        <v>0.85901551631888695</v>
       </c>
       <c r="G25">
         <f>F25-E25</f>
-        <v>-0.17730496453900702</v>
+        <v>-0.12564651328696208</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C26" t="s">
         <v>2</v>
@@ -1775,22 +1777,22 @@
         <v>3</v>
       </c>
       <c r="E26">
-        <v>0.97635933806146502</v>
+        <v>0.98492955234528201</v>
       </c>
       <c r="F26">
-        <v>0.79905437352245801</v>
+        <v>0.85928303905831904</v>
       </c>
       <c r="G26">
         <f>F26-E26</f>
-        <v>-0.17730496453900702</v>
+        <v>-0.12564651328696297</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C27" t="s">
         <v>2</v>
@@ -1799,22 +1801,22 @@
         <v>3</v>
       </c>
       <c r="E27">
-        <v>0.97399527186761203</v>
+        <v>0.98546459782414797</v>
       </c>
       <c r="F27">
-        <v>0.79669030732860502</v>
+        <v>0.859818084537185</v>
       </c>
       <c r="G27">
         <f>F27-E27</f>
-        <v>-0.17730496453900702</v>
+        <v>-0.12564651328696297</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C28" t="s">
         <v>2</v>
@@ -1823,22 +1825,22 @@
         <v>3</v>
       </c>
       <c r="E28">
-        <v>0.97635933806146502</v>
+        <v>0.984572855359372</v>
       </c>
       <c r="F28">
-        <v>0.79905437352245801</v>
+        <v>0.85892634207240903</v>
       </c>
       <c r="G28">
         <f>F28-E28</f>
-        <v>-0.17730496453900702</v>
+        <v>-0.12564651328696297</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C29" t="s">
         <v>2</v>
@@ -1847,22 +1849,22 @@
         <v>3</v>
       </c>
       <c r="E29">
-        <v>0.97635933806146502</v>
+        <v>0.98448368111289397</v>
       </c>
       <c r="F29">
-        <v>0.79905437352245801</v>
+        <v>0.858837167825931</v>
       </c>
       <c r="G29">
         <f>F29-E29</f>
-        <v>-0.17730496453900702</v>
+        <v>-0.12564651328696297</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="C30" t="s">
         <v>2</v>
@@ -1871,22 +1873,22 @@
         <v>3</v>
       </c>
       <c r="E30">
-        <v>0.97399527186761203</v>
+        <v>0.98430533261993902</v>
       </c>
       <c r="F30">
-        <v>0.79669030732860502</v>
+        <v>0.85865881933297605</v>
       </c>
       <c r="G30">
         <f>F30-E30</f>
-        <v>-0.17730496453900702</v>
+        <v>-0.12564651328696297</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="C31" t="s">
         <v>2</v>
@@ -1895,22 +1897,22 @@
         <v>3</v>
       </c>
       <c r="E31">
-        <v>0.97635933806146502</v>
+        <v>0.984572855359372</v>
       </c>
       <c r="F31">
-        <v>0.79905437352245801</v>
+        <v>0.85892634207240903</v>
       </c>
       <c r="G31">
         <f>F31-E31</f>
-        <v>-0.17730496453900702</v>
+        <v>-0.12564651328696297</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>92</v>
       </c>
       <c r="B32" t="s">
-        <v>41</v>
+        <v>93</v>
       </c>
       <c r="C32" t="s">
         <v>2</v>
@@ -1919,22 +1921,22 @@
         <v>3</v>
       </c>
       <c r="E32">
-        <v>0.97714736012608305</v>
+        <v>0.984572855359372</v>
       </c>
       <c r="F32">
-        <v>0.79984239558707604</v>
+        <v>0.85892634207240903</v>
       </c>
       <c r="G32">
         <f>F32-E32</f>
-        <v>-0.17730496453900702</v>
+        <v>-0.12564651328696297</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="B33" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="C33" t="s">
         <v>2</v>
@@ -1943,22 +1945,22 @@
         <v>3</v>
       </c>
       <c r="E33">
-        <v>0.97635933806146502</v>
+        <v>0.98501872659176004</v>
       </c>
       <c r="F33">
-        <v>0.79905437352245801</v>
+        <v>0.85937221330479696</v>
       </c>
       <c r="G33">
         <f>F33-E33</f>
-        <v>-0.17730496453900702</v>
+        <v>-0.12564651328696308</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C34" t="s">
         <v>2</v>
@@ -1967,22 +1969,22 @@
         <v>3</v>
       </c>
       <c r="E34">
-        <v>0.97557131599684699</v>
+        <v>0.98448229733345205</v>
       </c>
       <c r="F34">
-        <v>0.79826635145783997</v>
+        <v>0.85882457861410799</v>
       </c>
       <c r="G34">
         <f>F34-E34</f>
-        <v>-0.17730496453900702</v>
+        <v>-0.12565771871934406</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B35" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="C35" t="s">
         <v>2</v>
@@ -1991,22 +1993,22 @@
         <v>3</v>
       </c>
       <c r="E35">
-        <v>0.97635933806146502</v>
+        <v>0.98448229733345205</v>
       </c>
       <c r="F35">
-        <v>0.79905437352245801</v>
+        <v>0.85882457861410799</v>
       </c>
       <c r="G35">
         <f>F35-E35</f>
-        <v>-0.17730496453900702</v>
+        <v>-0.12565771871934406</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="B36" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
       <c r="C36" t="s">
         <v>2</v>
@@ -2015,22 +2017,22 @@
         <v>3</v>
       </c>
       <c r="E36">
-        <v>0.97399527186761203</v>
+        <v>0.98430253300035597</v>
       </c>
       <c r="F36">
-        <v>0.79669030732860502</v>
+        <v>0.85863360684980305</v>
       </c>
       <c r="G36">
         <f>F36-E36</f>
-        <v>-0.17730496453900702</v>
+        <v>-0.12566892615055292</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="B37" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="C37" t="s">
         <v>2</v>
@@ -2039,22 +2041,22 @@
         <v>3</v>
       </c>
       <c r="E37">
-        <v>0.97635933806146502</v>
+        <v>0.98510391579698497</v>
       </c>
       <c r="F37">
-        <v>0.79905437352245801</v>
+        <v>0.85942378021585897</v>
       </c>
       <c r="G37">
         <f>F37-E37</f>
-        <v>-0.17730496453900702</v>
+        <v>-0.12568013558112601</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="B38" t="s">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="C38" t="s">
         <v>2</v>
@@ -2063,22 +2065,22 @@
         <v>3</v>
       </c>
       <c r="E38">
-        <v>0.97635933806146502</v>
+        <v>0.98492148465381801</v>
       </c>
       <c r="F38">
-        <v>0.79905437352245801</v>
+        <v>0.85920770877944297</v>
       </c>
       <c r="G38">
         <f>F38-E38</f>
-        <v>-0.17730496453900702</v>
+        <v>-0.12571377587437504</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="B39" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="C39" t="s">
         <v>2</v>
@@ -2087,22 +2089,22 @@
         <v>3</v>
       </c>
       <c r="E39">
-        <v>0.97635933806146502</v>
+        <v>0.98492148465381801</v>
       </c>
       <c r="F39">
-        <v>0.79905437352245801</v>
+        <v>0.85920770877944297</v>
       </c>
       <c r="G39">
         <f>F39-E39</f>
-        <v>-0.17730496453900702</v>
+        <v>-0.12571377587437504</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="B40" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="C40" t="s">
         <v>2</v>
@@ -2111,22 +2113,22 @@
         <v>3</v>
       </c>
       <c r="E40">
-        <v>0.97557131599684699</v>
+        <v>0.98429693076374003</v>
       </c>
       <c r="F40">
-        <v>0.79826635145783997</v>
+        <v>0.85858315488936399</v>
       </c>
       <c r="G40">
         <f>F40-E40</f>
-        <v>-0.17730496453900702</v>
+        <v>-0.12571377587437604</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="B41" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="C41" t="s">
         <v>2</v>
@@ -2135,22 +2137,22 @@
         <v>3</v>
       </c>
       <c r="E41">
-        <v>0.97714736012608305</v>
+        <v>0.98492013919871502</v>
       </c>
       <c r="F41">
-        <v>0.79984239558707604</v>
+        <v>0.85919514589096102</v>
       </c>
       <c r="G41">
         <f>F41-E41</f>
-        <v>-0.17730496453900702</v>
+        <v>-0.125724993307754</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B42" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C42" t="s">
         <v>2</v>
@@ -2159,22 +2161,22 @@
         <v>3</v>
       </c>
       <c r="E42">
-        <v>0.97557131599684699</v>
+        <v>0.98492013919871502</v>
       </c>
       <c r="F42">
-        <v>0.79826635145783997</v>
+        <v>0.85919514589096102</v>
       </c>
       <c r="G42">
         <f>F42-E42</f>
-        <v>-0.17730496453900702</v>
+        <v>-0.125724993307754</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B43" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C43" t="s">
         <v>2</v>
@@ -2183,22 +2185,22 @@
         <v>3</v>
       </c>
       <c r="E43">
-        <v>0.97635933806146502</v>
+        <v>0.98429552957972699</v>
       </c>
       <c r="F43">
-        <v>0.79905437352245801</v>
+        <v>0.858570536271972</v>
       </c>
       <c r="G43">
         <f>F43-E43</f>
-        <v>-0.17730496453900702</v>
+        <v>-0.125724993307755</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>78</v>
+        <v>32</v>
       </c>
       <c r="B44" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
       <c r="C44" t="s">
         <v>2</v>
@@ -2207,22 +2209,22 @@
         <v>3</v>
       </c>
       <c r="E44">
-        <v>0.973207249802994</v>
+        <v>0.98436522826766704</v>
       </c>
       <c r="F44">
-        <v>0.79590228526398699</v>
+        <v>0.85848298043419902</v>
       </c>
       <c r="G44">
         <f>F44-E44</f>
-        <v>-0.17730496453900702</v>
+        <v>-0.12588224783346802</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
       <c r="B45" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
       <c r="C45" t="s">
         <v>2</v>
@@ -2231,22 +2233,22 @@
         <v>3</v>
       </c>
       <c r="E45">
-        <v>0.97635933806146502</v>
+        <v>0.98498391133357099</v>
       </c>
       <c r="F45">
-        <v>0.79905437352245801</v>
+        <v>0.85904540579191901</v>
       </c>
       <c r="G45">
         <f>F45-E45</f>
-        <v>-0.17730496453900702</v>
+        <v>-0.12593850554165198</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B46" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="C46" t="s">
         <v>2</v>
@@ -2255,22 +2257,22 @@
         <v>3</v>
       </c>
       <c r="E46">
-        <v>0.97635933806146502</v>
+        <v>0.98435824097247004</v>
       </c>
       <c r="F46">
-        <v>0.79905437352245801</v>
+        <v>0.85841973543081795</v>
       </c>
       <c r="G46">
         <f>F46-E46</f>
-        <v>-0.17730496453900702</v>
+        <v>-0.12593850554165209</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>92</v>
+        <v>24</v>
       </c>
       <c r="B47" t="s">
-        <v>93</v>
+        <v>25</v>
       </c>
       <c r="C47" t="s">
         <v>2</v>
@@ -2279,22 +2281,22 @@
         <v>3</v>
       </c>
       <c r="E47">
-        <v>0.97635933806146502</v>
+        <v>0.98489047831917698</v>
       </c>
       <c r="F47">
-        <v>0.79905437352245801</v>
+        <v>0.85891819400983405</v>
       </c>
       <c r="G47">
         <f>F47-E47</f>
-        <v>-0.17730496453900702</v>
+        <v>-0.12597228430934293</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>94</v>
+        <v>66</v>
       </c>
       <c r="B48" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="C48" t="s">
         <v>2</v>
@@ -2303,14 +2305,14 @@
         <v>3</v>
       </c>
       <c r="E48">
-        <v>0.97635933806146502</v>
+        <v>0.98681318681318597</v>
       </c>
       <c r="F48">
-        <v>0.79905437352245801</v>
+        <v>0.85924908424908397</v>
       </c>
       <c r="G48">
         <f>F48-E48</f>
-        <v>-0.17730496453900702</v>
+        <v>-0.127564102564102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove double gap penalty
</commit_message>
<xml_diff>
--- a/kuzmin analysis/Nearest Neighbor/human_CoV2_sims.xlsx
+++ b/kuzmin analysis/Nearest Neighbor/human_CoV2_sims.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NBOLLIG\Desktop\machine-mutation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2CE21B0A-2E1F-4C54-BBD4-042FFC350510}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{89B6CED4-0FF9-439C-8C0F-803284AA6AE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="human_CoV2_sims" sheetId="1" r:id="rId1"/>
@@ -1163,7 +1163,7 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,10 +1189,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -1201,22 +1201,22 @@
         <v>3</v>
       </c>
       <c r="E2">
-        <v>0.98514450346628202</v>
+        <v>0.98422090729782996</v>
       </c>
       <c r="F2">
-        <v>0.86206896551724099</v>
+        <v>0.85771920387305001</v>
       </c>
       <c r="G2">
         <f>F2-E2</f>
-        <v>-0.12307553794904103</v>
+        <v>-0.12650170342477995</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -1225,14 +1225,14 @@
         <v>3</v>
       </c>
       <c r="E3">
-        <v>0.99275634995296302</v>
+        <v>0.98514450346628202</v>
       </c>
       <c r="F3">
-        <v>0.86895578551269903</v>
+        <v>0.85783739983794005</v>
       </c>
       <c r="G3">
         <f>F3-E3</f>
-        <v>-0.12380056444026399</v>
+        <v>-0.12730710362834197</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1252,19 +1252,19 @@
         <v>0.98482399425287304</v>
       </c>
       <c r="F4">
-        <v>0.86054238505747105</v>
+        <v>0.85748922413793105</v>
       </c>
       <c r="G4">
         <f>F4-E4</f>
-        <v>-0.12428160919540199</v>
+        <v>-0.12733477011494199</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -1273,14 +1273,14 @@
         <v>3</v>
       </c>
       <c r="E5">
-        <v>0.98422090729782996</v>
+        <v>0.99275634995296302</v>
       </c>
       <c r="F5">
-        <v>0.85933297471758996</v>
+        <v>0.86528692380056405</v>
       </c>
       <c r="G5">
         <f>F5-E5</f>
-        <v>-0.12488793258024</v>
+        <v>-0.12746942615239898</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1300,11 +1300,11 @@
         <v>0.98341506910387799</v>
       </c>
       <c r="F6">
-        <v>0.858493089612126</v>
+        <v>0.85483727151136801</v>
       </c>
       <c r="G6">
         <f>F6-E6</f>
-        <v>-0.12492197949175199</v>
+        <v>-0.12857779759250998</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1324,11 +1324,11 @@
         <v>0.98403780988050604</v>
       </c>
       <c r="F7">
-        <v>0.85910469056536398</v>
+        <v>0.85544854645978197</v>
       </c>
       <c r="G7">
         <f>F7-E7</f>
-        <v>-0.12493311931514206</v>
+        <v>-0.12858926342072408</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1348,11 +1348,11 @@
         <v>0.98457010346057705</v>
       </c>
       <c r="F8">
-        <v>0.85961469853728101</v>
+        <v>0.85595790224759105</v>
       </c>
       <c r="G8">
         <f>F8-E8</f>
-        <v>-0.12495540492329604</v>
+        <v>-0.128612201212986</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1372,11 +1372,11 @@
         <v>0.98457010346057705</v>
       </c>
       <c r="F9">
-        <v>0.85961469853728101</v>
+        <v>0.85595790224759105</v>
       </c>
       <c r="G9">
         <f>F9-E9</f>
-        <v>-0.12495540492329604</v>
+        <v>-0.128612201212986</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1396,11 +1396,11 @@
         <v>0.98376449598572702</v>
       </c>
       <c r="F10">
-        <v>0.85878679750222997</v>
+        <v>0.855129348795718</v>
       </c>
       <c r="G10">
         <f>F10-E10</f>
-        <v>-0.12497769848349705</v>
+        <v>-0.12863514719000901</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1420,11 +1420,11 @@
         <v>0.98421475073575304</v>
       </c>
       <c r="F11">
-        <v>0.85918130741104004</v>
+        <v>0.85552483724248596</v>
       </c>
       <c r="G11">
         <f>F11-E11</f>
-        <v>-0.125033443324713</v>
+        <v>-0.12868991349326708</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1444,19 +1444,19 @@
         <v>0.98490397498883397</v>
       </c>
       <c r="F12">
-        <v>0.85984814649397001</v>
+        <v>0.85618579723090604</v>
       </c>
       <c r="G12">
         <f>F12-E12</f>
-        <v>-0.12505582849486396</v>
+        <v>-0.12871817775792793</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>88</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>89</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
@@ -1465,22 +1465,22 @@
         <v>3</v>
       </c>
       <c r="E13">
-        <v>0.98448229733345205</v>
+        <v>0.98489047831917698</v>
       </c>
       <c r="F13">
-        <v>0.85918130741104004</v>
+        <v>0.85605721949038804</v>
       </c>
       <c r="G13">
         <f>F13-E13</f>
-        <v>-0.12530098992241201</v>
+        <v>-0.12883325882878893</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
@@ -1489,22 +1489,22 @@
         <v>3</v>
       </c>
       <c r="E14">
-        <v>0.984572855359372</v>
+        <v>0.98492148465381801</v>
       </c>
       <c r="F14">
-        <v>0.85919386481184201</v>
+        <v>0.85608493932905005</v>
       </c>
       <c r="G14">
         <f>F14-E14</f>
-        <v>-0.12537899054752999</v>
+        <v>-0.12883654532476796</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>89</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
@@ -1516,19 +1516,19 @@
         <v>0.98448229733345205</v>
       </c>
       <c r="F15">
-        <v>0.859092125211807</v>
+        <v>0.85552483724248596</v>
       </c>
       <c r="G15">
         <f>F15-E15</f>
-        <v>-0.12539017212164505</v>
+        <v>-0.12895746009096609</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="B16" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
@@ -1537,22 +1537,22 @@
         <v>3</v>
       </c>
       <c r="E16">
-        <v>0.98369129311113002</v>
+        <v>0.984572855359372</v>
       </c>
       <c r="F16">
-        <v>0.858123161928526</v>
+        <v>0.85553772070626</v>
       </c>
       <c r="G16">
         <f>F16-E16</f>
-        <v>-0.12556813118260401</v>
+        <v>-0.129035134653112</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -1561,22 +1561,22 @@
         <v>3</v>
       </c>
       <c r="E17">
-        <v>0.98395292859053196</v>
+        <v>0.98448229733345205</v>
       </c>
       <c r="F17">
-        <v>0.85834001961308704</v>
+        <v>0.85543565504325303</v>
       </c>
       <c r="G17">
         <f>F17-E17</f>
-        <v>-0.12561290897744493</v>
+        <v>-0.12904664229019902</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="C18" t="s">
         <v>2</v>
@@ -1585,22 +1585,22 @@
         <v>3</v>
       </c>
       <c r="E18">
-        <v>0.98412981455064197</v>
+        <v>0.98369129311113002</v>
       </c>
       <c r="F18">
-        <v>0.85850570613409405</v>
+        <v>0.85446929863648502</v>
       </c>
       <c r="G18">
         <f>F18-E18</f>
-        <v>-0.12562410841654792</v>
+        <v>-0.129221994474645</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>90</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>91</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
@@ -1609,22 +1609,22 @@
         <v>3</v>
       </c>
       <c r="E19">
-        <v>0.98412981455064197</v>
+        <v>0.98395292859053196</v>
       </c>
       <c r="F19">
-        <v>0.85850570613409405</v>
+        <v>0.85468485334759703</v>
       </c>
       <c r="G19">
         <f>F19-E19</f>
-        <v>-0.12562410841654792</v>
+        <v>-0.12926807524293493</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="C20" t="s">
         <v>2</v>
@@ -1633,22 +1633,22 @@
         <v>3</v>
       </c>
       <c r="E20">
-        <v>0.98439728958630501</v>
+        <v>0.98377318116975698</v>
       </c>
       <c r="F20">
-        <v>0.85877318116975698</v>
+        <v>0.85449358059914404</v>
       </c>
       <c r="G20">
         <f>F20-E20</f>
-        <v>-0.12562410841654803</v>
+        <v>-0.12927960057061294</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>75</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
@@ -1657,22 +1657,22 @@
         <v>3</v>
       </c>
       <c r="E21">
-        <v>0.98377318116975698</v>
+        <v>0.98412981455064197</v>
       </c>
       <c r="F21">
-        <v>0.85814907275320895</v>
+        <v>0.85485021398002803</v>
       </c>
       <c r="G21">
         <f>F21-E21</f>
-        <v>-0.12562410841654803</v>
+        <v>-0.12927960057061394</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>6</v>
+        <v>90</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>91</v>
       </c>
       <c r="C22" t="s">
         <v>2</v>
@@ -1681,22 +1681,22 @@
         <v>3</v>
       </c>
       <c r="E22">
-        <v>0.98439589835042296</v>
+        <v>0.98412981455064197</v>
       </c>
       <c r="F22">
-        <v>0.85876058849754699</v>
+        <v>0.85485021398002803</v>
       </c>
       <c r="G22">
         <f>F22-E22</f>
-        <v>-0.12563530985287596</v>
+        <v>-0.12927960057061394</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
@@ -1705,22 +1705,22 @@
         <v>3</v>
       </c>
       <c r="E23">
-        <v>0.98457423094070395</v>
+        <v>0.98439728958630501</v>
       </c>
       <c r="F23">
-        <v>0.85893892108782799</v>
+        <v>0.85511768901569096</v>
       </c>
       <c r="G23">
         <f>F23-E23</f>
-        <v>-0.12563530985287596</v>
+        <v>-0.12927960057061405</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>76</v>
+        <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="C24" t="s">
         <v>2</v>
@@ -1729,22 +1729,22 @@
         <v>3</v>
       </c>
       <c r="E24">
-        <v>0.98448506464556396</v>
+        <v>0.98439589835042296</v>
       </c>
       <c r="F24">
-        <v>0.85884975479268799</v>
+        <v>0.85510477039679</v>
       </c>
       <c r="G24">
         <f>F24-E24</f>
-        <v>-0.12563530985287596</v>
+        <v>-0.12929112795363296</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>87</v>
+        <v>31</v>
       </c>
       <c r="C25" t="s">
         <v>2</v>
@@ -1753,22 +1753,22 @@
         <v>3</v>
       </c>
       <c r="E25">
-        <v>0.98466202960584903</v>
+        <v>0.98457423094070395</v>
       </c>
       <c r="F25">
-        <v>0.85901551631888695</v>
+        <v>0.85528310298707</v>
       </c>
       <c r="G25">
         <f>F25-E25</f>
-        <v>-0.12564651328696208</v>
+        <v>-0.12929112795363396</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="B26" t="s">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="C26" t="s">
         <v>2</v>
@@ -1777,14 +1777,14 @@
         <v>3</v>
       </c>
       <c r="E26">
-        <v>0.98492955234528201</v>
+        <v>0.98448506464556396</v>
       </c>
       <c r="F26">
-        <v>0.85928303905831904</v>
+        <v>0.85519393669193</v>
       </c>
       <c r="G26">
         <f>F26-E26</f>
-        <v>-0.12564651328696297</v>
+        <v>-0.12929112795363396</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1804,19 +1804,19 @@
         <v>0.98546459782414797</v>
       </c>
       <c r="F27">
-        <v>0.859818084537185</v>
+        <v>0.85616194043160299</v>
       </c>
       <c r="G27">
         <f>F27-E27</f>
-        <v>-0.12564651328696297</v>
+        <v>-0.12930265739254498</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="C28" t="s">
         <v>2</v>
@@ -1825,22 +1825,22 @@
         <v>3</v>
       </c>
       <c r="E28">
-        <v>0.984572855359372</v>
+        <v>0.98492955234528201</v>
       </c>
       <c r="F28">
-        <v>0.85892634207240903</v>
+        <v>0.85562689495273703</v>
       </c>
       <c r="G28">
         <f>F28-E28</f>
-        <v>-0.12564651328696297</v>
+        <v>-0.12930265739254498</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="B29" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="C29" t="s">
         <v>2</v>
@@ -1849,22 +1849,22 @@
         <v>3</v>
       </c>
       <c r="E29">
-        <v>0.98448368111289397</v>
+        <v>0.98466202960584903</v>
       </c>
       <c r="F29">
-        <v>0.858837167825931</v>
+        <v>0.85535937221330405</v>
       </c>
       <c r="G29">
         <f>F29-E29</f>
-        <v>-0.12564651328696297</v>
+        <v>-0.12930265739254498</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C30" t="s">
         <v>2</v>
@@ -1873,14 +1873,14 @@
         <v>3</v>
       </c>
       <c r="E30">
-        <v>0.98430533261993902</v>
+        <v>0.984572855359372</v>
       </c>
       <c r="F30">
-        <v>0.85865881933297605</v>
+        <v>0.85527019796682702</v>
       </c>
       <c r="G30">
         <f>F30-E30</f>
-        <v>-0.12564651328696297</v>
+        <v>-0.12930265739254498</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1900,11 +1900,11 @@
         <v>0.984572855359372</v>
       </c>
       <c r="F31">
-        <v>0.85892634207240903</v>
+        <v>0.85527019796682702</v>
       </c>
       <c r="G31">
         <f>F31-E31</f>
-        <v>-0.12564651328696297</v>
+        <v>-0.12930265739254498</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1924,19 +1924,19 @@
         <v>0.984572855359372</v>
       </c>
       <c r="F32">
-        <v>0.85892634207240903</v>
+        <v>0.85527019796682702</v>
       </c>
       <c r="G32">
         <f>F32-E32</f>
-        <v>-0.12564651328696297</v>
+        <v>-0.12930265739254498</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="C33" t="s">
         <v>2</v>
@@ -1945,22 +1945,22 @@
         <v>3</v>
       </c>
       <c r="E33">
-        <v>0.98501872659176004</v>
+        <v>0.98448368111289397</v>
       </c>
       <c r="F33">
-        <v>0.85937221330479696</v>
+        <v>0.85518102372034899</v>
       </c>
       <c r="G33">
         <f>F33-E33</f>
-        <v>-0.12564651328696308</v>
+        <v>-0.12930265739254498</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="C34" t="s">
         <v>2</v>
@@ -1969,22 +1969,22 @@
         <v>3</v>
       </c>
       <c r="E34">
-        <v>0.98448229733345205</v>
+        <v>0.98430533261993902</v>
       </c>
       <c r="F34">
-        <v>0.85882457861410799</v>
+        <v>0.85500267522739404</v>
       </c>
       <c r="G34">
         <f>F34-E34</f>
-        <v>-0.12565771871934406</v>
+        <v>-0.12930265739254498</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="C35" t="s">
         <v>2</v>
@@ -1996,19 +1996,19 @@
         <v>0.98448229733345205</v>
       </c>
       <c r="F35">
-        <v>0.85882457861410799</v>
+        <v>0.85516810844555402</v>
       </c>
       <c r="G35">
         <f>F35-E35</f>
-        <v>-0.12565771871934406</v>
+        <v>-0.12931418888789803</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="B36" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="C36" t="s">
         <v>2</v>
@@ -2017,22 +2017,22 @@
         <v>3</v>
       </c>
       <c r="E36">
-        <v>0.98430253300035597</v>
+        <v>0.98448229733345205</v>
       </c>
       <c r="F36">
-        <v>0.85863360684980305</v>
+        <v>0.85516810844555402</v>
       </c>
       <c r="G36">
         <f>F36-E36</f>
-        <v>-0.12566892615055292</v>
+        <v>-0.12931418888789803</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="B37" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="C37" t="s">
         <v>2</v>
@@ -2041,22 +2041,22 @@
         <v>3</v>
       </c>
       <c r="E37">
-        <v>0.98510391579698497</v>
+        <v>0.98430253300035597</v>
       </c>
       <c r="F37">
-        <v>0.85942378021585897</v>
+        <v>0.85497681056011399</v>
       </c>
       <c r="G37">
         <f>F37-E37</f>
-        <v>-0.12568013558112601</v>
+        <v>-0.12932572244024199</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="B38" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="C38" t="s">
         <v>2</v>
@@ -2065,14 +2065,14 @@
         <v>3</v>
       </c>
       <c r="E38">
-        <v>0.98492148465381801</v>
+        <v>0.98510391579698497</v>
       </c>
       <c r="F38">
-        <v>0.85920770877944297</v>
+        <v>0.85576665774685501</v>
       </c>
       <c r="G38">
         <f>F38-E38</f>
-        <v>-0.12571377587437504</v>
+        <v>-0.12933725805012997</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -2092,11 +2092,11 @@
         <v>0.98492148465381801</v>
       </c>
       <c r="F39">
-        <v>0.85920770877944297</v>
+        <v>0.85554960742326902</v>
       </c>
       <c r="G39">
         <f>F39-E39</f>
-        <v>-0.12571377587437504</v>
+        <v>-0.12937187723054899</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -2116,11 +2116,11 @@
         <v>0.98429693076374003</v>
       </c>
       <c r="F40">
-        <v>0.85858315488936399</v>
+        <v>0.85492505353319004</v>
       </c>
       <c r="G40">
         <f>F40-E40</f>
-        <v>-0.12571377587437604</v>
+        <v>-0.12937187723054999</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -2140,11 +2140,11 @@
         <v>0.98492013919871502</v>
       </c>
       <c r="F41">
-        <v>0.85919514589096102</v>
+        <v>0.85553671812260101</v>
       </c>
       <c r="G41">
         <f>F41-E41</f>
-        <v>-0.125724993307754</v>
+        <v>-0.129383421076114</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -2164,11 +2164,11 @@
         <v>0.98492013919871502</v>
       </c>
       <c r="F42">
-        <v>0.85919514589096102</v>
+        <v>0.85553671812260101</v>
       </c>
       <c r="G42">
         <f>F42-E42</f>
-        <v>-0.125724993307754</v>
+        <v>-0.129383421076114</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -2188,11 +2188,11 @@
         <v>0.98429552957972699</v>
       </c>
       <c r="F43">
-        <v>0.858570536271972</v>
+        <v>0.85491210850361299</v>
       </c>
       <c r="G43">
         <f>F43-E43</f>
-        <v>-0.125724993307755</v>
+        <v>-0.129383421076114</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -2212,11 +2212,11 @@
         <v>0.98436522826766704</v>
       </c>
       <c r="F44">
-        <v>0.85848298043419902</v>
+        <v>0.85481997677119603</v>
       </c>
       <c r="G44">
         <f>F44-E44</f>
-        <v>-0.12588224783346802</v>
+        <v>-0.129545251496471</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -2236,11 +2236,11 @@
         <v>0.98498391133357099</v>
       </c>
       <c r="F45">
-        <v>0.85904540579191901</v>
+        <v>0.85538076510547001</v>
       </c>
       <c r="G45">
         <f>F45-E45</f>
-        <v>-0.12593850554165198</v>
+        <v>-0.12960314622810098</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -2260,19 +2260,19 @@
         <v>0.98435824097247004</v>
       </c>
       <c r="F46">
-        <v>0.85841973543081795</v>
+        <v>0.85475509474436895</v>
       </c>
       <c r="G46">
         <f>F46-E46</f>
-        <v>-0.12593850554165209</v>
+        <v>-0.1296031462281011</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="B47" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="C47" t="s">
         <v>2</v>
@@ -2281,22 +2281,22 @@
         <v>3</v>
       </c>
       <c r="E47">
-        <v>0.98489047831917698</v>
+        <v>0.98681318681318597</v>
       </c>
       <c r="F47">
-        <v>0.85891819400983405</v>
+        <v>0.85714285714285698</v>
       </c>
       <c r="G47">
         <f>F47-E47</f>
-        <v>-0.12597228430934293</v>
+        <v>-0.12967032967032899</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B48" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C48" t="s">
         <v>2</v>
@@ -2305,14 +2305,14 @@
         <v>3</v>
       </c>
       <c r="E48">
-        <v>0.98681318681318597</v>
+        <v>0.98501872659176004</v>
       </c>
       <c r="F48">
-        <v>0.85924908424908397</v>
+        <v>0.85527019796682702</v>
       </c>
       <c r="G48">
         <f>F48-E48</f>
-        <v>-0.127564102564102</v>
+        <v>-0.12974852862493302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>